<commit_message>
Commit 03.1. Tema: estadisticos descriptivos II
</commit_message>
<xml_diff>
--- a/Datos/Raw/grupo_edad_altura_excel.xlsx
+++ b/Datos/Raw/grupo_edad_altura_excel.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/795fdf3ed47e8380/Trabajo/Academia/Anahuac/Cursos/Analisis_datos_I/R_ejercicios/Datos/Raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="349" documentId="13_ncr:1_{0EAC5EE9-CFCC-3641-AA7D-7120F92E1C72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3EF05316-F907-4AD7-800E-6B3F0043A9F6}"/>
+  <xr:revisionPtr revIDLastSave="472" documentId="13_ncr:1_{0EAC5EE9-CFCC-3641-AA7D-7120F92E1C72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D7094B1A-2D8F-45D1-B264-F67870D1112B}"/>
   <bookViews>
-    <workbookView xWindow="31425" yWindow="1095" windowWidth="22770" windowHeight="17970" activeTab="7" xr2:uid="{1B651967-EA38-4532-9886-F809CFA26B0F}"/>
+    <workbookView xWindow="27405" yWindow="420" windowWidth="22770" windowHeight="17340" xr2:uid="{1B651967-EA38-4532-9886-F809CFA26B0F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Altura" sheetId="1" r:id="rId1"/>
+    <sheet name="Posicion" sheetId="1" r:id="rId1"/>
     <sheet name="Edad" sheetId="2" r:id="rId2"/>
-    <sheet name="Moda" sheetId="4" r:id="rId3"/>
-    <sheet name="Mediana" sheetId="3" r:id="rId4"/>
+    <sheet name="Mediana" sheetId="3" r:id="rId3"/>
+    <sheet name="Moda" sheetId="4" r:id="rId4"/>
     <sheet name="Media" sheetId="5" r:id="rId5"/>
     <sheet name="Media_ponderada" sheetId="6" r:id="rId6"/>
     <sheet name="Media_geometrica" sheetId="7" r:id="rId7"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="109">
   <si>
     <t>Nombre</t>
   </si>
@@ -587,20 +587,40 @@
     <t>H =</t>
   </si>
   <si>
-    <t>Tiempo de recorrido</t>
+    <t>Mediana (n impar)</t>
+  </si>
+  <si>
+    <t>Mediana (n par)</t>
+  </si>
+  <si>
+    <t>Promedio</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Recuento</t>
+  </si>
+  <si>
+    <t>Concepto</t>
+  </si>
+  <si>
+    <t>Tiempo de recorrido
+(hr)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="6">
+  <numFmts count="7">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="167" formatCode="0.00000"/>
     <numFmt numFmtId="168" formatCode="0.0000"/>
     <numFmt numFmtId="169" formatCode="0.000"/>
     <numFmt numFmtId="170" formatCode="0.000%"/>
     <numFmt numFmtId="172" formatCode="0.00000000"/>
+    <numFmt numFmtId="177" formatCode="#,##0.0000000"/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -669,7 +689,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -703,12 +723,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -784,7 +798,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -842,10 +856,9 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -875,8 +888,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -939,22 +951,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -967,6 +969,9 @@
     <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1001,6 +1006,63 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1202,7 +1264,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>23812</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="680314" cy="346570"/>
@@ -1715,15 +1777,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94296A84-70D6-4841-8188-81D6440188F2}">
   <dimension ref="A1:P28"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1:E28"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="0" hidden="1" customWidth="1"/>
   </cols>
@@ -1805,16 +1867,16 @@
       <c r="F3" s="2">
         <v>2</v>
       </c>
-      <c r="I3" s="37">
+      <c r="I3" s="36">
         <v>1</v>
       </c>
-      <c r="J3" s="37">
+      <c r="J3" s="36">
         <v>1.5740000000000001</v>
       </c>
-      <c r="K3" s="37">
+      <c r="K3" s="36">
         <v>10</v>
       </c>
-      <c r="L3" s="37">
+      <c r="L3" s="36">
         <v>1.5740000000000001</v>
       </c>
     </row>
@@ -1837,10 +1899,10 @@
       <c r="F4" s="2">
         <v>3</v>
       </c>
-      <c r="I4" s="37"/>
-      <c r="J4" s="37"/>
-      <c r="K4" s="37"/>
-      <c r="L4" s="37"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="36"/>
+      <c r="L4" s="36"/>
       <c r="O4" s="18" t="s">
         <v>41</v>
       </c>
@@ -2379,10 +2441,10 @@
         <v>25</v>
       </c>
       <c r="G26" s="11"/>
-      <c r="I26" s="37">
+      <c r="I26" s="36">
         <v>9</v>
       </c>
-      <c r="J26" s="38">
+      <c r="J26" s="37">
         <v>1.8</v>
       </c>
       <c r="L26">
@@ -2409,8 +2471,8 @@
         <v>26</v>
       </c>
       <c r="G27" s="11"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="38"/>
+      <c r="I27" s="36"/>
+      <c r="J27" s="37"/>
     </row>
     <row r="28" spans="1:12">
       <c r="A28" s="1">
@@ -2459,11 +2521,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBD45052-C1E2-4A4A-9E82-BCE0932FCA6C}">
   <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14:G15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -2750,10 +2814,10 @@
       <c r="E14">
         <v>13</v>
       </c>
-      <c r="F14" s="39" t="s">
+      <c r="F14" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="G14" s="39">
+      <c r="G14" s="38">
         <f>+(19+20)/2</f>
         <v>19.5</v>
       </c>
@@ -2774,8 +2838,8 @@
       <c r="E15">
         <v>14</v>
       </c>
-      <c r="F15" s="39"/>
-      <c r="G15" s="39"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="1">
@@ -2994,12 +3058,694 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50721B54-C4AD-CC41-9C2F-5E16BAF72E49}">
+  <dimension ref="A1:H31"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="8.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="33" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" s="33" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="85" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="85" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="86" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="85" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="85" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="86" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="86" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="87" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="87" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="87">
+        <v>19</v>
+      </c>
+      <c r="E3" s="89" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="89" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="89">
+        <v>19</v>
+      </c>
+      <c r="H3" s="90">
+        <v>1.54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="30">
+        <v>18</v>
+      </c>
+      <c r="E4" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="31">
+        <v>18</v>
+      </c>
+      <c r="H4" s="91">
+        <v>1.55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="30">
+        <v>19</v>
+      </c>
+      <c r="E5" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="31">
+        <v>19</v>
+      </c>
+      <c r="H5" s="91">
+        <v>1.58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="30">
+        <v>19</v>
+      </c>
+      <c r="E6" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" s="31">
+        <v>19</v>
+      </c>
+      <c r="H6" s="91">
+        <v>1.58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="30">
+        <v>20</v>
+      </c>
+      <c r="E7" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" s="31">
+        <v>20</v>
+      </c>
+      <c r="H7" s="91">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="30">
+        <v>18</v>
+      </c>
+      <c r="E8" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="31">
+        <v>18</v>
+      </c>
+      <c r="H8" s="91">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="30">
+        <v>20</v>
+      </c>
+      <c r="E9" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="G9" s="31">
+        <v>20</v>
+      </c>
+      <c r="H9" s="92">
+        <v>1.63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="30">
+        <v>18</v>
+      </c>
+      <c r="E10" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" s="31">
+        <v>18</v>
+      </c>
+      <c r="H10" s="92">
+        <v>1.65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="30">
+        <v>20</v>
+      </c>
+      <c r="E11" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" s="31">
+        <v>20</v>
+      </c>
+      <c r="H11" s="92">
+        <v>1.66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="30">
+        <v>21</v>
+      </c>
+      <c r="E12" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" s="31">
+        <v>21</v>
+      </c>
+      <c r="H12" s="92">
+        <v>1.66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="30">
+        <v>20</v>
+      </c>
+      <c r="E13" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" s="31">
+        <v>20</v>
+      </c>
+      <c r="H13" s="92">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="30">
+        <v>18</v>
+      </c>
+      <c r="E14" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" s="31">
+        <v>18</v>
+      </c>
+      <c r="H14" s="92">
+        <v>1.68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="30">
+        <v>18</v>
+      </c>
+      <c r="E15" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" s="31">
+        <v>18</v>
+      </c>
+      <c r="H15" s="92">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="30">
+        <v>21</v>
+      </c>
+      <c r="E16" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" s="31">
+        <v>21</v>
+      </c>
+      <c r="H16" s="92">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="30">
+        <v>19</v>
+      </c>
+      <c r="E17" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="G17" s="31">
+        <v>19</v>
+      </c>
+      <c r="H17" s="92">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="30">
+        <v>20</v>
+      </c>
+      <c r="E18" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="F18" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="G18" s="31">
+        <v>20</v>
+      </c>
+      <c r="H18" s="92">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="30">
+        <v>21</v>
+      </c>
+      <c r="E19" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="G19" s="31">
+        <v>21</v>
+      </c>
+      <c r="H19" s="92">
+        <v>1.72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="30">
+        <v>22</v>
+      </c>
+      <c r="E20" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="F20" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="G20" s="31">
+        <v>22</v>
+      </c>
+      <c r="H20" s="92">
+        <v>1.72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="30">
+        <v>18</v>
+      </c>
+      <c r="E21" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="G21" s="31">
+        <v>18</v>
+      </c>
+      <c r="H21" s="92">
+        <v>1.74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="30">
+        <v>19</v>
+      </c>
+      <c r="E22" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="F22" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="G22" s="31">
+        <v>19</v>
+      </c>
+      <c r="H22" s="92">
+        <v>1.74</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="30">
+        <v>20</v>
+      </c>
+      <c r="E23" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="G23" s="31">
+        <v>20</v>
+      </c>
+      <c r="H23" s="92">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="30">
+        <v>20</v>
+      </c>
+      <c r="E24" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="G24" s="31">
+        <v>20</v>
+      </c>
+      <c r="H24" s="92">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="30">
+        <v>19</v>
+      </c>
+      <c r="E25" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="F25" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="G25" s="31">
+        <v>19</v>
+      </c>
+      <c r="H25" s="92">
+        <v>1.77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" s="30">
+        <v>28</v>
+      </c>
+      <c r="E26" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="F26" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="G26" s="31">
+        <v>28</v>
+      </c>
+      <c r="H26" s="92">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" s="30">
+        <v>19</v>
+      </c>
+      <c r="E27" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="F27" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="G27" s="31">
+        <v>19</v>
+      </c>
+      <c r="H27" s="92">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="88" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="88" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="88">
+        <v>23</v>
+      </c>
+      <c r="E28" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="F28" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="G28" s="31">
+        <v>23</v>
+      </c>
+      <c r="H28" s="92">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="E29" s="93" t="s">
+        <v>29</v>
+      </c>
+      <c r="F29" s="93" t="s">
+        <v>6</v>
+      </c>
+      <c r="G29" s="93">
+        <v>21</v>
+      </c>
+      <c r="H29" s="94">
+        <v>1.83</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="B31" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31" s="33">
+        <f>MEDIAN(C3:C28)</f>
+        <v>19.5</v>
+      </c>
+      <c r="F31" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="G31" s="33">
+        <f>MEDIAN(G3:G29)</f>
+        <v>20</v>
+      </c>
+      <c r="H31" s="33">
+        <f>MEDIAN(H3:H29)</f>
+        <v>1.7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{128A430F-44B8-4346-BD95-009EC474D597}">
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3647,422 +4393,23 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50721B54-C4AD-CC41-9C2F-5E16BAF72E49}">
-  <dimension ref="A1:F27"/>
-  <sheetViews>
-    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="1">
-        <v>44428.412731481483</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2">
-        <v>19</v>
-      </c>
-      <c r="F2">
-        <f>MEDIAN(D2:D27)</f>
-        <v>19.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="1">
-        <v>44428.411574074074</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="1">
-        <v>44428.390196759261</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="1">
-        <v>44428.38753472222</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="1">
-        <v>44428.387071759258</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="1">
-        <v>44428.387025462966</v>
-      </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="1">
-        <v>44428.387997685182</v>
-      </c>
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="1">
-        <v>44428.391886574071</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="1">
-        <v>44428.387685185182</v>
-      </c>
-      <c r="B10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="1">
-        <v>44428.412407407406</v>
-      </c>
-      <c r="B11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="1">
-        <v>44428.387129629627</v>
-      </c>
-      <c r="B12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="1">
-        <v>44428.387314814812</v>
-      </c>
-      <c r="B13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="1">
-        <v>44428.390590277777</v>
-      </c>
-      <c r="B14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="1">
-        <v>44428.387175925927</v>
-      </c>
-      <c r="B15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="1">
-        <v>44428.387199074074</v>
-      </c>
-      <c r="B16" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="1">
-        <v>44428.386747685188</v>
-      </c>
-      <c r="B17" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="1">
-        <v>44428.38721064815</v>
-      </c>
-      <c r="B18" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="1">
-        <v>44428.412210648145</v>
-      </c>
-      <c r="B19" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="1">
-        <v>44428.38685185185</v>
-      </c>
-      <c r="B20" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="1">
-        <v>44428.387314814812</v>
-      </c>
-      <c r="B21" t="s">
-        <v>25</v>
-      </c>
-      <c r="C21" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="1">
-        <v>44428.387118055558</v>
-      </c>
-      <c r="B22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C22" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="1">
-        <v>44428.388182870367</v>
-      </c>
-      <c r="B23" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="1">
-        <v>44428.386886574073</v>
-      </c>
-      <c r="B24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C24" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="1">
-        <v>44428.387199074074</v>
-      </c>
-      <c r="B25" t="s">
-        <v>19</v>
-      </c>
-      <c r="C25" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="1">
-        <v>44428.414803240739</v>
-      </c>
-      <c r="B26" t="s">
-        <v>27</v>
-      </c>
-      <c r="C26" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="1">
-        <v>44428.412442129629</v>
-      </c>
-      <c r="B27" t="s">
-        <v>30</v>
-      </c>
-      <c r="C27" t="s">
-        <v>6</v>
-      </c>
-      <c r="D27">
-        <v>23</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{014CA872-2210-C546-AE16-7299B6E99820}">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
+    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G6" sqref="G6:I6"/>
+      <selection pane="bottomLeft" activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
+    <col min="8" max="8" width="29.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="11" t="s">
         <v>64</v>
       </c>
@@ -4072,20 +4419,24 @@
       <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="95" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="F1" s="95"/>
+      <c r="H1" s="96" t="s">
+        <v>107</v>
+      </c>
+      <c r="I1" s="96" t="s">
         <v>66</v>
       </c>
-      <c r="I1" s="19" t="s">
+      <c r="J1" s="96" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:10">
       <c r="A2" s="11">
         <v>1</v>
       </c>
@@ -4101,8 +4452,12 @@
       <c r="E2" s="20">
         <v>1.54</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="18.75">
+      <c r="F2" s="20"/>
+      <c r="H2" s="87"/>
+      <c r="I2" s="87"/>
+      <c r="J2" s="87"/>
+    </row>
+    <row r="3" spans="1:10" ht="18.75">
       <c r="A3" s="11">
         <v>2</v>
       </c>
@@ -4116,21 +4471,22 @@
         <v>18</v>
       </c>
       <c r="E3" s="20">
-        <v>2.1</v>
-      </c>
-      <c r="G3" s="27" t="s">
+        <v>1.55</v>
+      </c>
+      <c r="F3" s="20"/>
+      <c r="H3" s="97" t="s">
         <v>63</v>
       </c>
-      <c r="H3">
+      <c r="I3" s="30">
         <f>+SUM(D2:D28)</f>
         <v>538</v>
       </c>
-      <c r="I3" s="3">
+      <c r="J3" s="43">
         <f>SUM(E2:E28)</f>
-        <v>49.129999999999988</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+        <v>45.619999999999983</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="11">
         <v>3</v>
       </c>
@@ -4144,21 +4500,22 @@
         <v>19</v>
       </c>
       <c r="E4" s="20">
-        <v>2.1</v>
-      </c>
-      <c r="G4" s="18" t="s">
+        <v>1.58</v>
+      </c>
+      <c r="F4" s="20"/>
+      <c r="H4" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="H4">
+      <c r="I4" s="30">
         <f>+COUNT(D2:D28)</f>
         <v>27</v>
       </c>
-      <c r="I4">
+      <c r="J4" s="30">
         <f>COUNT(E2:E28)</f>
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:10">
       <c r="A5" s="11">
         <v>4</v>
       </c>
@@ -4172,10 +4529,14 @@
         <v>19</v>
       </c>
       <c r="E5" s="20">
-        <v>2.1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>1.58</v>
+      </c>
+      <c r="F5" s="20"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="30"/>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="11">
         <v>5</v>
       </c>
@@ -4189,21 +4550,22 @@
         <v>20</v>
       </c>
       <c r="E6" s="20">
-        <v>2.1</v>
-      </c>
-      <c r="G6" s="18" t="s">
+        <v>1.6</v>
+      </c>
+      <c r="F6" s="20"/>
+      <c r="H6" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="H6" s="28">
-        <f>+H3/H4</f>
+      <c r="I6" s="98">
+        <f>+I3/I4</f>
         <v>19.925925925925927</v>
       </c>
-      <c r="I6" s="28">
-        <f>+I3/I4</f>
-        <v>1.8196296296296293</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="J6" s="98">
+        <f>+J3/J4</f>
+        <v>1.6896296296296289</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" s="11">
         <v>6</v>
       </c>
@@ -4217,16 +4579,18 @@
         <v>18</v>
       </c>
       <c r="E7" s="20">
-        <v>2.1</v>
-      </c>
-      <c r="H7" s="3">
+        <v>1.6</v>
+      </c>
+      <c r="F7" s="20"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="43">
         <v>19.925925925925899</v>
       </c>
-      <c r="I7" s="3">
+      <c r="J7" s="43">
         <v>1.6896296296296289</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:10">
       <c r="A8" s="11">
         <v>7</v>
       </c>
@@ -4239,11 +4603,15 @@
       <c r="D8">
         <v>20</v>
       </c>
-      <c r="E8" s="22">
-        <v>2.1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="E8" s="20">
+        <v>1.63</v>
+      </c>
+      <c r="F8" s="22"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="30"/>
+      <c r="J8" s="30"/>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="11">
         <v>8</v>
       </c>
@@ -4257,21 +4625,22 @@
         <v>18</v>
       </c>
       <c r="E9" s="20">
-        <v>2.1</v>
-      </c>
-      <c r="G9" s="18" t="s">
+        <v>1.65</v>
+      </c>
+      <c r="F9" s="20"/>
+      <c r="H9" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="H9" s="6">
+      <c r="I9" s="99">
         <f>+MIN(D2:D28)</f>
         <v>18</v>
       </c>
-      <c r="I9" s="3">
+      <c r="J9" s="43">
         <f>+MIN(E2:E28)</f>
         <v>1.54</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:10">
       <c r="A10" s="11">
         <v>9</v>
       </c>
@@ -4287,19 +4656,20 @@
       <c r="E10" s="20">
         <v>1.66</v>
       </c>
-      <c r="G10" s="18" t="s">
+      <c r="F10" s="20"/>
+      <c r="H10" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="H10" s="6">
+      <c r="I10" s="99">
         <f>+MAX(D2:D28)</f>
         <v>28</v>
       </c>
-      <c r="I10" s="3">
+      <c r="J10" s="43">
         <f>+MAX(E2:E28)</f>
-        <v>2.1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+        <v>1.83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" s="11">
         <v>10</v>
       </c>
@@ -4315,8 +4685,12 @@
       <c r="E11" s="20">
         <v>1.66</v>
       </c>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="F11" s="20"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="30"/>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="11">
         <v>11</v>
       </c>
@@ -4332,19 +4706,20 @@
       <c r="E12" s="20">
         <v>1.67</v>
       </c>
-      <c r="G12" s="18" t="s">
+      <c r="F12" s="20"/>
+      <c r="H12" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="H12" s="3">
-        <f>+H9-H6</f>
+      <c r="I12" s="43">
+        <f>+I9-I6</f>
         <v>-1.9259259259259274</v>
       </c>
-      <c r="I12" s="3">
-        <f>+I9-I6</f>
-        <v>-0.27962962962962923</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="J12" s="43">
+        <f>+J9-J6</f>
+        <v>-0.14962962962962889</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" s="11">
         <v>12</v>
       </c>
@@ -4360,19 +4735,20 @@
       <c r="E13" s="20">
         <v>1.68</v>
       </c>
-      <c r="G13" s="18" t="s">
+      <c r="F13" s="20"/>
+      <c r="H13" s="100" t="s">
         <v>71</v>
       </c>
-      <c r="H13" s="3">
-        <f>+H10-H6</f>
+      <c r="I13" s="101">
+        <f>+I10-I6</f>
         <v>8.0740740740740726</v>
       </c>
-      <c r="I13" s="3">
-        <f>+I10-I6</f>
-        <v>0.28037037037037082</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+      <c r="J13" s="101">
+        <f>+J10-J6</f>
+        <v>0.14037037037037114</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" s="11">
         <v>13</v>
       </c>
@@ -4388,8 +4764,9 @@
       <c r="E14" s="20">
         <v>1.7</v>
       </c>
-    </row>
-    <row r="15" spans="1:9">
+      <c r="F14" s="20"/>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" s="11">
         <v>14</v>
       </c>
@@ -4402,11 +4779,12 @@
       <c r="D15">
         <v>21</v>
       </c>
-      <c r="E15" s="22">
+      <c r="E15" s="20">
         <v>1.7</v>
       </c>
-    </row>
-    <row r="16" spans="1:9">
+      <c r="F15" s="22"/>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" s="11">
         <v>15</v>
       </c>
@@ -4422,8 +4800,9 @@
       <c r="E16" s="20">
         <v>1.7</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="F16" s="20"/>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" s="11">
         <v>16</v>
       </c>
@@ -4439,8 +4818,9 @@
       <c r="E17" s="20">
         <v>1.7</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="F17" s="20"/>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" s="11">
         <v>17</v>
       </c>
@@ -4456,8 +4836,9 @@
       <c r="E18" s="20">
         <v>1.72</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="F18" s="20"/>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" s="11">
         <v>18</v>
       </c>
@@ -4473,8 +4854,9 @@
       <c r="E19" s="20">
         <v>1.72</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="F19" s="20"/>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" s="11">
         <v>19</v>
       </c>
@@ -4490,8 +4872,9 @@
       <c r="E20" s="20">
         <v>1.74</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="F20" s="20"/>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" s="11">
         <v>20</v>
       </c>
@@ -4507,8 +4890,9 @@
       <c r="E21" s="20">
         <v>1.74</v>
       </c>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="F21" s="20"/>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" s="11">
         <v>21</v>
       </c>
@@ -4524,8 +4908,9 @@
       <c r="E22" s="20">
         <v>1.75</v>
       </c>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="F22" s="20"/>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" s="11">
         <v>22</v>
       </c>
@@ -4541,8 +4926,9 @@
       <c r="E23" s="20">
         <v>1.75</v>
       </c>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="F23" s="20"/>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" s="11">
         <v>23</v>
       </c>
@@ -4558,8 +4944,9 @@
       <c r="E24" s="20">
         <v>1.77</v>
       </c>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="F24" s="20"/>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" s="11">
         <v>24</v>
       </c>
@@ -4575,8 +4962,9 @@
       <c r="E25" s="20">
         <v>1.8</v>
       </c>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="F25" s="20"/>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" s="11">
         <v>25</v>
       </c>
@@ -4592,8 +4980,9 @@
       <c r="E26" s="20">
         <v>1.8</v>
       </c>
-    </row>
-    <row r="27" spans="1:5">
+      <c r="F26" s="20"/>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" s="11">
         <v>26</v>
       </c>
@@ -4609,8 +4998,9 @@
       <c r="E27" s="20">
         <v>1.8</v>
       </c>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="F27" s="20"/>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" s="11">
         <v>27</v>
       </c>
@@ -4623,9 +5013,10 @@
       <c r="D28">
         <v>21</v>
       </c>
-      <c r="E28" s="22">
+      <c r="E28" s="20">
         <v>1.83</v>
       </c>
+      <c r="F28" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4637,7 +5028,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -4646,7 +5037,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="33" t="s">
         <v>72</v>
       </c>
     </row>
@@ -4656,104 +5047,104 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="33.75">
-      <c r="A3" s="65"/>
-      <c r="B3" s="66" t="s">
+      <c r="A3" s="63"/>
+      <c r="B3" s="64" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="64" t="s">
         <v>82</v>
       </c>
-      <c r="C3" s="66" t="s">
-        <v>80</v>
-      </c>
-      <c r="D3" s="67" t="s">
+      <c r="D3" s="65" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="68" t="s">
+      <c r="A4" s="102" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="44">
+      <c r="B4" s="103">
+        <v>10</v>
+      </c>
+      <c r="C4" s="72">
         <v>4</v>
       </c>
-      <c r="C4" s="44">
-        <v>10</v>
-      </c>
-      <c r="D4" s="44">
+      <c r="D4" s="72">
         <f>+B4*C4</f>
         <v>40</v>
       </c>
-      <c r="E4" s="31"/>
+      <c r="E4" s="30"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="104" t="s">
         <v>75</v>
       </c>
-      <c r="B5" s="31">
+      <c r="B5" s="105">
+        <v>9</v>
+      </c>
+      <c r="C5" s="73">
         <v>4</v>
       </c>
-      <c r="C5" s="31">
-        <v>10</v>
-      </c>
-      <c r="D5" s="31">
+      <c r="D5" s="73">
         <f t="shared" ref="D5:D7" si="0">+B5*C5</f>
-        <v>40</v>
-      </c>
-      <c r="E5" s="31"/>
+        <v>36</v>
+      </c>
+      <c r="E5" s="30"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="104" t="s">
         <v>76</v>
       </c>
-      <c r="B6" s="31">
+      <c r="B6" s="105">
+        <v>9</v>
+      </c>
+      <c r="C6" s="73">
         <v>4</v>
       </c>
-      <c r="C6" s="31">
-        <v>10</v>
-      </c>
-      <c r="D6" s="31">
+      <c r="D6" s="73">
         <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="E6" s="31"/>
+        <v>36</v>
+      </c>
+      <c r="E6" s="30"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="69" t="s">
+      <c r="A7" s="106" t="s">
         <v>77</v>
       </c>
-      <c r="B7" s="70">
+      <c r="B7" s="107">
+        <v>6.9</v>
+      </c>
+      <c r="C7" s="108">
         <v>18</v>
       </c>
-      <c r="C7" s="45">
-        <v>9</v>
-      </c>
-      <c r="D7" s="45">
+      <c r="D7" s="108">
         <f t="shared" si="0"/>
-        <v>162</v>
-      </c>
-      <c r="E7" s="31"/>
+        <v>124.2</v>
+      </c>
+      <c r="E7" s="30"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="67" t="s">
         <v>78</v>
       </c>
-      <c r="B8">
-        <f>SUM(B4:B7)</f>
+      <c r="B8" s="27">
+        <f>+SUM(B4:B7)</f>
+        <v>34.9</v>
+      </c>
+      <c r="C8" s="27">
+        <f>+SUM(C4:C7)</f>
         <v>30</v>
       </c>
-      <c r="C8">
-        <f>+SUM(C4:C7)</f>
-        <v>39</v>
-      </c>
-      <c r="D8" s="32">
+      <c r="D8" s="109">
         <f>+SUM(D4:D7)</f>
-        <v>282</v>
-      </c>
-      <c r="E8" s="31"/>
+        <v>236.2</v>
+      </c>
+      <c r="E8" s="30"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="E9" s="31"/>
+      <c r="E9" s="30"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="B10" s="71" t="s">
+      <c r="B10" s="66" t="s">
         <v>41</v>
       </c>
       <c r="C10" s="8">
@@ -4761,12 +5152,12 @@
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="B11" s="72" t="s">
+      <c r="B11" s="67" t="s">
         <v>79</v>
       </c>
-      <c r="C11" s="73">
-        <f>+C8/C10</f>
-        <v>9.75</v>
+      <c r="C11" s="110">
+        <f>+B8/C10</f>
+        <v>8.7249999999999996</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="9.9499999999999993" customHeight="1">
@@ -4774,36 +5165,36 @@
       <c r="C12" s="8"/>
     </row>
     <row r="13" spans="1:5" ht="18.75">
-      <c r="B13" s="33" t="s">
+      <c r="B13" s="32" t="s">
         <v>83</v>
       </c>
       <c r="C13" s="8">
         <f>+D8</f>
-        <v>282</v>
-      </c>
-      <c r="D13" s="74" t="s">
+        <v>236.2</v>
+      </c>
+      <c r="D13" s="68" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="18.75">
-      <c r="B14" s="33" t="s">
+      <c r="B14" s="32" t="s">
         <v>84</v>
       </c>
       <c r="C14" s="8">
-        <f>+B8</f>
+        <f>+C8</f>
         <v>30</v>
       </c>
-      <c r="D14" s="74" t="s">
+      <c r="D14" s="68" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="B15" s="72" t="s">
+      <c r="B15" s="67" t="s">
         <v>93</v>
       </c>
-      <c r="C15" s="73">
+      <c r="C15" s="110">
         <f>+C13/C14</f>
-        <v>9.4</v>
+        <v>7.8733333333333331</v>
       </c>
     </row>
   </sheetData>
@@ -4817,7 +5208,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -4832,177 +5223,177 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="45">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="42" t="s">
         <v>85</v>
       </c>
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="42" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="43" t="s">
+      <c r="C2" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="D2" s="43" t="s">
+      <c r="D2" s="42" t="s">
         <v>89</v>
       </c>
-      <c r="E2" s="43" t="s">
+      <c r="E2" s="42" t="s">
         <v>88</v>
       </c>
-      <c r="F2" s="43" t="s">
+      <c r="F2" s="42" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="47">
+      <c r="A3" s="45">
         <v>1</v>
       </c>
-      <c r="B3" s="48">
+      <c r="B3" s="46">
         <v>1000</v>
       </c>
-      <c r="C3" s="49">
+      <c r="C3" s="47">
         <v>4.6899999999999997E-2</v>
       </c>
-      <c r="D3" s="50">
+      <c r="D3" s="48">
         <f>+B3*C3</f>
         <v>46.9</v>
       </c>
-      <c r="E3" s="51">
+      <c r="E3" s="49">
         <f>+B3+D3</f>
         <v>1046.9000000000001</v>
       </c>
-      <c r="F3" s="52">
+      <c r="F3" s="50">
         <f>1+C3</f>
         <v>1.0468999999999999</v>
       </c>
-      <c r="G3" s="40"/>
+      <c r="G3" s="39"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="53">
+      <c r="A4" s="51">
         <v>2</v>
       </c>
-      <c r="B4" s="54">
+      <c r="B4" s="52">
         <f>+E3</f>
         <v>1046.9000000000001</v>
       </c>
-      <c r="C4" s="55">
+      <c r="C4" s="53">
         <v>5.5E-2</v>
       </c>
-      <c r="D4" s="56">
+      <c r="D4" s="54">
         <f>+B4*C4</f>
         <v>57.579500000000003</v>
       </c>
-      <c r="E4" s="57">
+      <c r="E4" s="55">
         <f>+B4+D4</f>
         <v>1104.4795000000001</v>
       </c>
-      <c r="F4" s="58">
+      <c r="F4" s="56">
         <f t="shared" ref="F4:F6" si="0">1+C4</f>
         <v>1.0549999999999999</v>
       </c>
-      <c r="G4" s="40"/>
+      <c r="G4" s="39"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="53">
+      <c r="A5" s="51">
         <v>3</v>
       </c>
-      <c r="B5" s="54">
+      <c r="B5" s="52">
         <f>+E4</f>
         <v>1104.4795000000001</v>
       </c>
-      <c r="C5" s="55">
+      <c r="C5" s="53">
         <v>6.4199999999999993E-2</v>
       </c>
-      <c r="D5" s="56">
+      <c r="D5" s="54">
         <f>+B5*C5</f>
         <v>70.907583900000006</v>
       </c>
-      <c r="E5" s="57">
+      <c r="E5" s="55">
         <f>+B5+D5</f>
         <v>1175.3870839000001</v>
       </c>
-      <c r="F5" s="58">
+      <c r="F5" s="56">
         <f t="shared" si="0"/>
         <v>1.0642</v>
       </c>
-      <c r="G5" s="40"/>
+      <c r="G5" s="39"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="59">
+      <c r="A6" s="57">
         <v>4</v>
       </c>
-      <c r="B6" s="60">
+      <c r="B6" s="58">
         <f>+E5</f>
         <v>1175.3870839000001</v>
       </c>
-      <c r="C6" s="61">
+      <c r="C6" s="59">
         <v>4.2700000000000002E-2</v>
       </c>
-      <c r="D6" s="62">
+      <c r="D6" s="60">
         <f>+B6*C6</f>
         <v>50.189028482530006</v>
       </c>
-      <c r="E6" s="63">
+      <c r="E6" s="61">
         <f>+B6+D6</f>
         <v>1225.57611238253</v>
       </c>
-      <c r="F6" s="64">
+      <c r="F6" s="62">
         <f t="shared" si="0"/>
         <v>1.0427</v>
       </c>
-      <c r="G6" s="40"/>
+      <c r="G6" s="39"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="C8" s="46"/>
+      <c r="C8" s="44"/>
       <c r="D8" s="18"/>
       <c r="E8" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="F8" s="46"/>
-      <c r="G8" s="40"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="39"/>
     </row>
     <row r="10" spans="1:7">
       <c r="A10">
         <v>1</v>
       </c>
-      <c r="B10" s="35">
+      <c r="B10" s="34">
         <v>1000</v>
       </c>
-      <c r="C10" s="42"/>
+      <c r="C10" s="41"/>
       <c r="D10" s="3"/>
-      <c r="E10" s="35"/>
+      <c r="E10" s="111"/>
       <c r="F10" s="3"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11">
         <v>2</v>
       </c>
-      <c r="B11" s="35"/>
-      <c r="C11" s="42"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="41"/>
       <c r="D11" s="3"/>
-      <c r="E11" s="35"/>
+      <c r="E11" s="34"/>
     </row>
     <row r="12" spans="1:7">
       <c r="A12">
         <v>3</v>
       </c>
-      <c r="B12" s="35"/>
-      <c r="C12" s="42"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="41"/>
       <c r="D12" s="3"/>
-      <c r="E12" s="35"/>
+      <c r="E12" s="34"/>
     </row>
     <row r="13" spans="1:7">
       <c r="A13">
         <v>4</v>
       </c>
-      <c r="B13" s="35"/>
-      <c r="C13" s="42"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="41"/>
       <c r="D13" s="3"/>
-      <c r="E13" s="35"/>
+      <c r="E13" s="34"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="E14" s="36"/>
+      <c r="E14" s="35"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="B15" s="36"/>
+      <c r="B15" s="35"/>
       <c r="D15" s="3"/>
     </row>
   </sheetData>
@@ -5013,137 +5404,135 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B682753-6962-4871-9D9A-D4D9AA98E97D}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18.75">
-      <c r="A1" s="89" t="s">
+      <c r="A1" s="84" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30">
-      <c r="A2" s="80" t="s">
+    <row r="2" spans="1:4" ht="45">
+      <c r="A2" s="75" t="s">
         <v>99</v>
       </c>
-      <c r="B2" s="81" t="s">
+      <c r="B2" s="76" t="s">
         <v>96</v>
       </c>
-      <c r="C2" s="81" t="s">
+      <c r="C2" s="76" t="s">
         <v>97</v>
       </c>
-      <c r="D2" s="82" t="s">
-        <v>102</v>
+      <c r="D2" s="77" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="83" t="s">
+      <c r="A3" s="78" t="s">
         <v>98</v>
       </c>
-      <c r="B3" s="83">
+      <c r="B3" s="78">
         <v>90</v>
       </c>
-      <c r="C3" s="84">
+      <c r="C3" s="79">
         <f>1/B3</f>
         <v>1.1111111111111112E-2</v>
       </c>
-      <c r="D3" s="85"/>
+      <c r="D3" s="80"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="78" t="s">
+      <c r="A4" s="73" t="s">
         <v>98</v>
       </c>
-      <c r="B4" s="78">
+      <c r="B4" s="73">
         <v>70</v>
       </c>
-      <c r="C4" s="79">
+      <c r="C4" s="74">
         <f t="shared" ref="C4:C7" si="0">1/B4</f>
         <v>1.4285714285714285E-2</v>
       </c>
-      <c r="D4" s="56"/>
+      <c r="D4" s="54"/>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="78" t="s">
+      <c r="A5" s="73" t="s">
         <v>98</v>
       </c>
-      <c r="B5" s="78">
+      <c r="B5" s="73">
         <v>45</v>
       </c>
-      <c r="C5" s="79">
+      <c r="C5" s="74">
         <f t="shared" si="0"/>
         <v>2.2222222222222223E-2</v>
       </c>
-      <c r="D5" s="56"/>
+      <c r="D5" s="54"/>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="78" t="s">
+      <c r="A6" s="73" t="s">
         <v>98</v>
       </c>
-      <c r="B6" s="78">
+      <c r="B6" s="73">
         <v>40</v>
       </c>
-      <c r="C6" s="79">
+      <c r="C6" s="74">
         <f t="shared" si="0"/>
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="D6" s="56"/>
+      <c r="D6" s="54"/>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="86" t="s">
+      <c r="A7" s="81" t="s">
         <v>98</v>
       </c>
-      <c r="B7" s="86">
+      <c r="B7" s="81">
         <v>50</v>
       </c>
-      <c r="C7" s="87">
+      <c r="C7" s="82">
         <f t="shared" si="0"/>
         <v>0.02</v>
       </c>
-      <c r="D7" s="88"/>
+      <c r="D7" s="83"/>
     </row>
     <row r="8" spans="1:4">
       <c r="D8" s="11"/>
     </row>
     <row r="9" spans="1:4">
-      <c r="B9" s="72" t="s">
+      <c r="D9" s="11"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="B10" s="67" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="41"/>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="B11" s="39"/>
-      <c r="C11" s="75">
-        <f>+SUM(C3:C7)</f>
-        <v>9.2619047619047615E-2</v>
-      </c>
+      <c r="C10" s="40"/>
     </row>
     <row r="12" spans="1:4">
-      <c r="B12" s="39"/>
-      <c r="C12" s="39"/>
-    </row>
-    <row r="14" spans="1:4" ht="15.75">
-      <c r="B14" s="76" t="s">
+      <c r="B12" s="38"/>
+      <c r="C12" s="69"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="B13" s="38"/>
+      <c r="C13" s="38"/>
+    </row>
+    <row r="15" spans="1:4" ht="15.75">
+      <c r="B15" s="70" t="s">
         <v>101</v>
       </c>
-      <c r="C14" s="77">
-        <f>5/C11</f>
-        <v>53.984575835475582</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="C16" s="3"/>
+      <c r="C15" s="71"/>
+    </row>
+    <row r="17" spans="3:3">
+      <c r="C17" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Commit 4. Reorganizar archivos y aumento de ignore
</commit_message>
<xml_diff>
--- a/Datos/Raw/grupo_edad_altura_excel.xlsx
+++ b/Datos/Raw/grupo_edad_altura_excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/795fdf3ed47e8380/Trabajo/Academia/Anahuac/Cursos/Analisis_datos_I/R_ejercicios/Datos/Raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="472" documentId="13_ncr:1_{0EAC5EE9-CFCC-3641-AA7D-7120F92E1C72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D7094B1A-2D8F-45D1-B264-F67870D1112B}"/>
+  <xr:revisionPtr revIDLastSave="631" documentId="13_ncr:1_{0EAC5EE9-CFCC-3641-AA7D-7120F92E1C72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3991B577-A813-864A-93A9-68EA4799C2E8}"/>
   <bookViews>
-    <workbookView xWindow="27405" yWindow="420" windowWidth="22770" windowHeight="17340" xr2:uid="{1B651967-EA38-4532-9886-F809CFA26B0F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="7" xr2:uid="{1B651967-EA38-4532-9886-F809CFA26B0F}"/>
   </bookViews>
   <sheets>
     <sheet name="Posicion" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="113">
   <si>
     <t>Nombre</t>
   </si>
@@ -593,20 +593,32 @@
     <t>Mediana (n par)</t>
   </si>
   <si>
-    <t>Promedio</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>Recuento</t>
-  </si>
-  <si>
     <t>Concepto</t>
   </si>
   <si>
     <t>Tiempo de recorrido
 (hr)</t>
+  </si>
+  <si>
+    <t>Media geométrica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 / x </t>
+  </si>
+  <si>
+    <t>Cuando X =&gt; 0</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>1/x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t = </t>
+  </si>
+  <si>
+    <t>Velocidad promedio</t>
   </si>
 </sst>
 </file>
@@ -615,14 +627,14 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="7">
     <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="167" formatCode="0.00000"/>
-    <numFmt numFmtId="168" formatCode="0.0000"/>
-    <numFmt numFmtId="169" formatCode="0.000"/>
-    <numFmt numFmtId="170" formatCode="0.000%"/>
-    <numFmt numFmtId="172" formatCode="0.00000000"/>
-    <numFmt numFmtId="177" formatCode="#,##0.0000000"/>
+    <numFmt numFmtId="165" formatCode="0.00000"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="169" formatCode="0.00000000"/>
+    <numFmt numFmtId="177" formatCode="0.0000%"/>
+    <numFmt numFmtId="178" formatCode="0.00000%"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -689,7 +701,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -726,8 +738,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -793,12 +811,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -873,23 +900,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -905,7 +925,7 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -923,7 +943,7 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -938,10 +958,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -960,9 +977,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -975,7 +989,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -990,7 +1004,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -999,7 +1013,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1062,7 +1076,46 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1091,8 +1144,8 @@
       <xdr:rowOff>216236</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="383674" cy="256674"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="CuadroTexto 1">
@@ -1186,7 +1239,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="CuadroTexto 1">
@@ -1268,8 +1321,8 @@
       <xdr:rowOff>23812</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="680314" cy="346570"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="CuadroTexto 1">
@@ -1311,6 +1364,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -1413,7 +1467,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="CuadroTexto 1">
@@ -1777,20 +1831,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94296A84-70D6-4841-8188-81D6440188F2}">
   <dimension ref="A1:P28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1:E28"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="30">
+    <row r="1" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>8</v>
       </c>
@@ -1828,7 +1882,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>44428.412731481483</v>
       </c>
@@ -1848,7 +1902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>44428.411574074074</v>
       </c>
@@ -1867,20 +1921,20 @@
       <c r="F3" s="2">
         <v>2</v>
       </c>
-      <c r="I3" s="36">
+      <c r="I3" s="106">
         <v>1</v>
       </c>
-      <c r="J3" s="36">
+      <c r="J3" s="106">
         <v>1.5740000000000001</v>
       </c>
-      <c r="K3" s="36">
+      <c r="K3" s="106">
         <v>10</v>
       </c>
-      <c r="L3" s="36">
+      <c r="L3" s="106">
         <v>1.5740000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>44428.390196759261</v>
       </c>
@@ -1899,10 +1953,10 @@
       <c r="F4" s="2">
         <v>3</v>
       </c>
-      <c r="I4" s="36"/>
-      <c r="J4" s="36"/>
-      <c r="K4" s="36"/>
-      <c r="L4" s="36"/>
+      <c r="I4" s="106"/>
+      <c r="J4" s="106"/>
+      <c r="K4" s="106"/>
+      <c r="L4" s="106"/>
       <c r="O4" s="18" t="s">
         <v>41</v>
       </c>
@@ -1910,7 +1964,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>44428.38753472222</v>
       </c>
@@ -1938,7 +1992,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>44428.387071759258</v>
       </c>
@@ -1968,7 +2022,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>44428.387025462966</v>
       </c>
@@ -1995,7 +2049,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>44428.387997685182</v>
       </c>
@@ -2022,7 +2076,7 @@
         <v>1.5828571428571425</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>44428.391886574071</v>
       </c>
@@ -2043,7 +2097,7 @@
       </c>
       <c r="G9" s="14"/>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>44428.387685185182</v>
       </c>
@@ -2065,7 +2119,7 @@
       <c r="G10" s="14"/>
       <c r="L10" s="3"/>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>44428.412407407406</v>
       </c>
@@ -2087,7 +2141,7 @@
       <c r="G11" s="14"/>
       <c r="L11" s="3"/>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>44428.387129629627</v>
       </c>
@@ -2109,7 +2163,7 @@
       <c r="G12" s="14"/>
       <c r="L12" s="3"/>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>44428.387314814812</v>
       </c>
@@ -2130,7 +2184,7 @@
       </c>
       <c r="G13" s="14"/>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>44428.390590277777</v>
       </c>
@@ -2151,7 +2205,7 @@
       </c>
       <c r="G14" s="14"/>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>44428.387175925927</v>
       </c>
@@ -2198,7 +2252,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>44428.387199074074</v>
       </c>
@@ -2219,7 +2273,7 @@
       </c>
       <c r="G16" s="14"/>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>44428.386747685188</v>
       </c>
@@ -2240,7 +2294,7 @@
       </c>
       <c r="G17" s="14"/>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>44428.38721064815</v>
       </c>
@@ -2261,7 +2315,7 @@
       </c>
       <c r="G18" s="14"/>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>44428.412210648145</v>
       </c>
@@ -2282,7 +2336,7 @@
       </c>
       <c r="G19" s="14"/>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>44428.38685185185</v>
       </c>
@@ -2303,7 +2357,7 @@
       </c>
       <c r="G20" s="14"/>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>44428.387314814812</v>
       </c>
@@ -2324,7 +2378,7 @@
       </c>
       <c r="G21" s="14"/>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>44428.387118055558</v>
       </c>
@@ -2358,7 +2412,7 @@
         <v>1.75</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>44428.388182870367</v>
       </c>
@@ -2379,7 +2433,7 @@
       </c>
       <c r="G23" s="11"/>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>44428.386886574073</v>
       </c>
@@ -2400,7 +2454,7 @@
       </c>
       <c r="G24" s="11"/>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>44428.387199074074</v>
       </c>
@@ -2421,7 +2475,7 @@
       </c>
       <c r="G25" s="11"/>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>44428.414803240739</v>
       </c>
@@ -2441,17 +2495,17 @@
         <v>25</v>
       </c>
       <c r="G26" s="11"/>
-      <c r="I26" s="36">
+      <c r="I26" s="106">
         <v>9</v>
       </c>
-      <c r="J26" s="37">
+      <c r="J26" s="107">
         <v>1.8</v>
       </c>
       <c r="L26">
         <v>25.2</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>44428.412442129629</v>
       </c>
@@ -2471,10 +2525,10 @@
         <v>26</v>
       </c>
       <c r="G27" s="11"/>
-      <c r="I27" s="36"/>
-      <c r="J27" s="37"/>
-    </row>
-    <row r="28" spans="1:12">
+      <c r="I27" s="106"/>
+      <c r="J27" s="107"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>44428.387476851851</v>
       </c>
@@ -2525,12 +2579,12 @@
       <selection activeCell="G14" sqref="G14:G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>8</v>
       </c>
@@ -2562,7 +2616,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>44428.411574074074</v>
       </c>
@@ -2589,7 +2643,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>44428.387025462966</v>
       </c>
@@ -2607,7 +2661,7 @@
       </c>
       <c r="K3" s="18"/>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>44428.391886574071</v>
       </c>
@@ -2631,7 +2685,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>44428.387314814812</v>
       </c>
@@ -2655,7 +2709,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>44428.390590277777</v>
       </c>
@@ -2679,7 +2733,7 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>44428.38685185185</v>
       </c>
@@ -2696,7 +2750,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>44428.412731481483</v>
       </c>
@@ -2713,7 +2767,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>44428.390196759261</v>
       </c>
@@ -2730,7 +2784,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>44428.38753472222</v>
       </c>
@@ -2747,7 +2801,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>44428.387199074074</v>
       </c>
@@ -2764,7 +2818,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>44428.387314814812</v>
       </c>
@@ -2781,7 +2835,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>44428.386886574073</v>
       </c>
@@ -2798,7 +2852,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>44428.414803240739</v>
       </c>
@@ -2814,15 +2868,15 @@
       <c r="E14">
         <v>13</v>
       </c>
-      <c r="F14" s="38" t="s">
+      <c r="F14" s="108" t="s">
         <v>54</v>
       </c>
-      <c r="G14" s="38">
+      <c r="G14" s="108">
         <f>+(19+20)/2</f>
         <v>19.5</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>44428.387071759258</v>
       </c>
@@ -2838,10 +2892,10 @@
       <c r="E15">
         <v>14</v>
       </c>
-      <c r="F15" s="38"/>
-      <c r="G15" s="38"/>
-    </row>
-    <row r="16" spans="1:14">
+      <c r="F15" s="108"/>
+      <c r="G15" s="108"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>44428.387997685182</v>
       </c>
@@ -2858,7 +2912,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>44428.387685185182</v>
       </c>
@@ -2875,7 +2929,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>44428.387129629627</v>
       </c>
@@ -2892,7 +2946,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>44428.386747685188</v>
       </c>
@@ -2909,7 +2963,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>44428.387118055558</v>
       </c>
@@ -2926,7 +2980,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>44428.388182870367</v>
       </c>
@@ -2943,7 +2997,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>44428.412407407406</v>
       </c>
@@ -2960,7 +3014,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>44428.387175925927</v>
       </c>
@@ -2977,7 +3031,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>44428.38721064815</v>
       </c>
@@ -2994,7 +3048,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>44428.412210648145</v>
       </c>
@@ -3011,7 +3065,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>44428.412442129629</v>
       </c>
@@ -3028,7 +3082,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>44428.387199074074</v>
       </c>
@@ -3066,12 +3120,12 @@
       <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="33" t="s">
         <v>103</v>
       </c>
@@ -3079,53 +3133,53 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="85" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="85" t="s">
+      <c r="B2" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="86" t="s">
+      <c r="C2" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="85" t="s">
+      <c r="E2" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="85" t="s">
+      <c r="F2" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="86" t="s">
+      <c r="G2" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="86" t="s">
+      <c r="H2" s="81" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="87" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="82" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="87" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="87">
+      <c r="B3" s="82" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="82">
         <v>19</v>
       </c>
-      <c r="E3" s="89" t="s">
+      <c r="E3" s="84" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="89" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="89">
+      <c r="F3" s="84" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="84">
         <v>19</v>
       </c>
-      <c r="H3" s="90">
+      <c r="H3" s="85">
         <v>1.54</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="30" t="s">
         <v>13</v>
       </c>
@@ -3144,11 +3198,11 @@
       <c r="G4" s="31">
         <v>18</v>
       </c>
-      <c r="H4" s="91">
+      <c r="H4" s="86">
         <v>1.55</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="30" t="s">
         <v>10</v>
       </c>
@@ -3167,11 +3221,11 @@
       <c r="G5" s="31">
         <v>19</v>
       </c>
-      <c r="H5" s="91">
+      <c r="H5" s="86">
         <v>1.58</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="30" t="s">
         <v>15</v>
       </c>
@@ -3190,11 +3244,11 @@
       <c r="G6" s="31">
         <v>19</v>
       </c>
-      <c r="H6" s="91">
+      <c r="H6" s="86">
         <v>1.58</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="30" t="s">
         <v>4</v>
       </c>
@@ -3213,11 +3267,11 @@
       <c r="G7" s="31">
         <v>20</v>
       </c>
-      <c r="H7" s="91">
+      <c r="H7" s="86">
         <v>1.6</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="30" t="s">
         <v>16</v>
       </c>
@@ -3236,11 +3290,11 @@
       <c r="G8" s="31">
         <v>18</v>
       </c>
-      <c r="H8" s="91">
+      <c r="H8" s="86">
         <v>1.6</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="30" t="s">
         <v>12</v>
       </c>
@@ -3259,11 +3313,11 @@
       <c r="G9" s="31">
         <v>20</v>
       </c>
-      <c r="H9" s="92">
+      <c r="H9" s="87">
         <v>1.63</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="30" t="s">
         <v>11</v>
       </c>
@@ -3282,11 +3336,11 @@
       <c r="G10" s="31">
         <v>18</v>
       </c>
-      <c r="H10" s="92">
+      <c r="H10" s="87">
         <v>1.65</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="30" t="s">
         <v>14</v>
       </c>
@@ -3305,11 +3359,11 @@
       <c r="G11" s="31">
         <v>20</v>
       </c>
-      <c r="H11" s="92">
+      <c r="H11" s="87">
         <v>1.66</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="30" t="s">
         <v>33</v>
       </c>
@@ -3328,11 +3382,11 @@
       <c r="G12" s="31">
         <v>21</v>
       </c>
-      <c r="H12" s="92">
+      <c r="H12" s="87">
         <v>1.66</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="30" t="s">
         <v>23</v>
       </c>
@@ -3351,11 +3405,11 @@
       <c r="G13" s="31">
         <v>20</v>
       </c>
-      <c r="H13" s="92">
+      <c r="H13" s="87">
         <v>1.67</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="30" t="s">
         <v>20</v>
       </c>
@@ -3374,11 +3428,11 @@
       <c r="G14" s="31">
         <v>18</v>
       </c>
-      <c r="H14" s="92">
+      <c r="H14" s="87">
         <v>1.68</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="30" t="s">
         <v>21</v>
       </c>
@@ -3397,11 +3451,11 @@
       <c r="G15" s="31">
         <v>18</v>
       </c>
-      <c r="H15" s="92">
+      <c r="H15" s="87">
         <v>1.7</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="30" t="s">
         <v>22</v>
       </c>
@@ -3420,11 +3474,11 @@
       <c r="G16" s="31">
         <v>21</v>
       </c>
-      <c r="H16" s="92">
+      <c r="H16" s="87">
         <v>1.7</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="30" t="s">
         <v>26</v>
       </c>
@@ -3443,11 +3497,11 @@
       <c r="G17" s="31">
         <v>19</v>
       </c>
-      <c r="H17" s="92">
+      <c r="H17" s="87">
         <v>1.7</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="30" t="s">
         <v>31</v>
       </c>
@@ -3466,11 +3520,11 @@
       <c r="G18" s="31">
         <v>20</v>
       </c>
-      <c r="H18" s="92">
+      <c r="H18" s="87">
         <v>1.7</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="30" t="s">
         <v>24</v>
       </c>
@@ -3489,11 +3543,11 @@
       <c r="G19" s="31">
         <v>21</v>
       </c>
-      <c r="H19" s="92">
+      <c r="H19" s="87">
         <v>1.72</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="30" t="s">
         <v>32</v>
       </c>
@@ -3512,11 +3566,11 @@
       <c r="G20" s="31">
         <v>22</v>
       </c>
-      <c r="H20" s="92">
+      <c r="H20" s="87">
         <v>1.72</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="30" t="s">
         <v>18</v>
       </c>
@@ -3535,11 +3589,11 @@
       <c r="G21" s="31">
         <v>18</v>
       </c>
-      <c r="H21" s="92">
+      <c r="H21" s="87">
         <v>1.74</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="30" t="s">
         <v>25</v>
       </c>
@@ -3558,11 +3612,11 @@
       <c r="G22" s="31">
         <v>19</v>
       </c>
-      <c r="H22" s="92">
+      <c r="H22" s="87">
         <v>1.74</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="30" t="s">
         <v>17</v>
       </c>
@@ -3581,11 +3635,11 @@
       <c r="G23" s="31">
         <v>20</v>
       </c>
-      <c r="H23" s="92">
+      <c r="H23" s="87">
         <v>1.75</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="30" t="s">
         <v>7</v>
       </c>
@@ -3604,11 +3658,11 @@
       <c r="G24" s="31">
         <v>20</v>
       </c>
-      <c r="H24" s="92">
+      <c r="H24" s="87">
         <v>1.75</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="30" t="s">
         <v>28</v>
       </c>
@@ -3627,11 +3681,11 @@
       <c r="G25" s="31">
         <v>19</v>
       </c>
-      <c r="H25" s="92">
+      <c r="H25" s="87">
         <v>1.77</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="30" t="s">
         <v>19</v>
       </c>
@@ -3650,11 +3704,11 @@
       <c r="G26" s="31">
         <v>28</v>
       </c>
-      <c r="H26" s="92">
+      <c r="H26" s="87">
         <v>1.8</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="30" t="s">
         <v>27</v>
       </c>
@@ -3673,18 +3727,18 @@
       <c r="G27" s="31">
         <v>19</v>
       </c>
-      <c r="H27" s="92">
+      <c r="H27" s="87">
         <v>1.8</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
-      <c r="A28" s="88" t="s">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="83" t="s">
         <v>30</v>
       </c>
-      <c r="B28" s="88" t="s">
-        <v>6</v>
-      </c>
-      <c r="C28" s="88">
+      <c r="B28" s="83" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="83">
         <v>23</v>
       </c>
       <c r="E28" s="31" t="s">
@@ -3696,25 +3750,25 @@
       <c r="G28" s="31">
         <v>23</v>
       </c>
-      <c r="H28" s="92">
+      <c r="H28" s="87">
         <v>1.8</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
-      <c r="E29" s="93" t="s">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E29" s="88" t="s">
         <v>29</v>
       </c>
-      <c r="F29" s="93" t="s">
-        <v>6</v>
-      </c>
-      <c r="G29" s="93">
+      <c r="F29" s="88" t="s">
+        <v>6</v>
+      </c>
+      <c r="G29" s="88">
         <v>21</v>
       </c>
-      <c r="H29" s="94">
+      <c r="H29" s="89">
         <v>1.83</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B31" s="28" t="s">
         <v>47</v>
       </c>
@@ -3748,13 +3802,13 @@
       <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="12.85546875" customWidth="1"/>
+    <col min="7" max="7" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="45">
+    <row r="1" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>62</v>
       </c>
@@ -3780,7 +3834,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2">
         <f>+COUNTIF($D$2:$D$28,D2)</f>
         <v>7</v>
@@ -3820,7 +3874,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3">
         <f t="shared" ref="A3:A28" si="0">+COUNTIF($D$2:$D$28,D3)</f>
         <v>6</v>
@@ -3841,7 +3895,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -3859,7 +3913,7 @@
         <v>1.58</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -3877,7 +3931,7 @@
         <v>1.58</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -3895,7 +3949,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -3920,7 +3974,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -3945,7 +3999,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -3963,7 +4017,7 @@
         <v>1.65</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -3987,7 +4041,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -4012,7 +4066,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -4037,7 +4091,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -4062,7 +4116,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -4087,7 +4141,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -4112,7 +4166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -4137,7 +4191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -4162,7 +4216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -4187,7 +4241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4212,7 +4266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -4237,7 +4291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -4262,7 +4316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -4280,7 +4334,7 @@
         <v>1.75</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -4298,7 +4352,7 @@
         <v>1.75</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -4316,7 +4370,7 @@
         <v>1.77</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4334,7 +4388,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -4352,7 +4406,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4370,7 +4424,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -4402,14 +4456,14 @@
       <selection pane="bottomLeft" activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" customWidth="1"/>
-    <col min="8" max="8" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.6640625" customWidth="1"/>
+    <col min="8" max="8" width="29.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>64</v>
       </c>
@@ -4419,24 +4473,24 @@
       <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="67" t="s">
+      <c r="D1" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="95" t="s">
+      <c r="E1" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="95"/>
-      <c r="H1" s="96" t="s">
-        <v>107</v>
-      </c>
-      <c r="I1" s="96" t="s">
+      <c r="F1" s="90"/>
+      <c r="H1" s="91" t="s">
+        <v>104</v>
+      </c>
+      <c r="I1" s="91" t="s">
         <v>66</v>
       </c>
-      <c r="J1" s="96" t="s">
+      <c r="J1" s="91" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="11">
         <v>1</v>
       </c>
@@ -4453,11 +4507,11 @@
         <v>1.54</v>
       </c>
       <c r="F2" s="20"/>
-      <c r="H2" s="87"/>
-      <c r="I2" s="87"/>
-      <c r="J2" s="87"/>
-    </row>
-    <row r="3" spans="1:10" ht="18.75">
+      <c r="H2" s="82"/>
+      <c r="I2" s="82"/>
+      <c r="J2" s="82"/>
+    </row>
+    <row r="3" spans="1:10" ht="17" x14ac:dyDescent="0.25">
       <c r="A3" s="11">
         <v>2</v>
       </c>
@@ -4474,19 +4528,19 @@
         <v>1.55</v>
       </c>
       <c r="F3" s="20"/>
-      <c r="H3" s="97" t="s">
+      <c r="H3" s="92" t="s">
         <v>63</v>
       </c>
       <c r="I3" s="30">
         <f>+SUM(D2:D28)</f>
         <v>538</v>
       </c>
-      <c r="J3" s="43">
+      <c r="J3" s="40">
         <f>SUM(E2:E28)</f>
         <v>45.619999999999983</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="11">
         <v>3</v>
       </c>
@@ -4515,7 +4569,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="11">
         <v>4</v>
       </c>
@@ -4536,7 +4590,7 @@
       <c r="I5" s="30"/>
       <c r="J5" s="30"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="11">
         <v>5</v>
       </c>
@@ -4556,16 +4610,16 @@
       <c r="H6" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="I6" s="98">
+      <c r="I6" s="93">
         <f>+I3/I4</f>
         <v>19.925925925925927</v>
       </c>
-      <c r="J6" s="98">
+      <c r="J6" s="93">
         <f>+J3/J4</f>
         <v>1.6896296296296289</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="11">
         <v>6</v>
       </c>
@@ -4583,14 +4637,14 @@
       </c>
       <c r="F7" s="20"/>
       <c r="H7" s="30"/>
-      <c r="I7" s="43">
+      <c r="I7" s="40">
         <v>19.925925925925899</v>
       </c>
-      <c r="J7" s="43">
+      <c r="J7" s="40">
         <v>1.6896296296296289</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="11">
         <v>7</v>
       </c>
@@ -4611,7 +4665,7 @@
       <c r="I8" s="30"/>
       <c r="J8" s="30"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="11">
         <v>8</v>
       </c>
@@ -4631,16 +4685,16 @@
       <c r="H9" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="I9" s="99">
+      <c r="I9" s="94">
         <f>+MIN(D2:D28)</f>
         <v>18</v>
       </c>
-      <c r="J9" s="43">
+      <c r="J9" s="40">
         <f>+MIN(E2:E28)</f>
         <v>1.54</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="11">
         <v>9</v>
       </c>
@@ -4660,16 +4714,16 @@
       <c r="H10" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="I10" s="99">
+      <c r="I10" s="94">
         <f>+MAX(D2:D28)</f>
         <v>28</v>
       </c>
-      <c r="J10" s="43">
+      <c r="J10" s="40">
         <f>+MAX(E2:E28)</f>
         <v>1.83</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="11">
         <v>10</v>
       </c>
@@ -4690,7 +4744,7 @@
       <c r="I11" s="30"/>
       <c r="J11" s="30"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
         <v>11</v>
       </c>
@@ -4710,16 +4764,16 @@
       <c r="H12" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="I12" s="43">
+      <c r="I12" s="40">
         <f>+I9-I6</f>
         <v>-1.9259259259259274</v>
       </c>
-      <c r="J12" s="43">
+      <c r="J12" s="40">
         <f>+J9-J6</f>
         <v>-0.14962962962962889</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="11">
         <v>12</v>
       </c>
@@ -4736,19 +4790,19 @@
         <v>1.68</v>
       </c>
       <c r="F13" s="20"/>
-      <c r="H13" s="100" t="s">
+      <c r="H13" s="95" t="s">
         <v>71</v>
       </c>
-      <c r="I13" s="101">
+      <c r="I13" s="96">
         <f>+I10-I6</f>
         <v>8.0740740740740726</v>
       </c>
-      <c r="J13" s="101">
+      <c r="J13" s="96">
         <f>+J10-J6</f>
         <v>0.14037037037037114</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="11">
         <v>13</v>
       </c>
@@ -4766,7 +4820,7 @@
       </c>
       <c r="F14" s="20"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="11">
         <v>14</v>
       </c>
@@ -4784,7 +4838,7 @@
       </c>
       <c r="F15" s="22"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="11">
         <v>15</v>
       </c>
@@ -4802,7 +4856,7 @@
       </c>
       <c r="F16" s="20"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="11">
         <v>16</v>
       </c>
@@ -4820,7 +4874,7 @@
       </c>
       <c r="F17" s="20"/>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="11">
         <v>17</v>
       </c>
@@ -4838,7 +4892,7 @@
       </c>
       <c r="F18" s="20"/>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="11">
         <v>18</v>
       </c>
@@ -4856,7 +4910,7 @@
       </c>
       <c r="F19" s="20"/>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="11">
         <v>19</v>
       </c>
@@ -4874,7 +4928,7 @@
       </c>
       <c r="F20" s="20"/>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="11">
         <v>20</v>
       </c>
@@ -4892,7 +4946,7 @@
       </c>
       <c r="F21" s="20"/>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="11">
         <v>21</v>
       </c>
@@ -4910,7 +4964,7 @@
       </c>
       <c r="F22" s="20"/>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="11">
         <v>22</v>
       </c>
@@ -4928,7 +4982,7 @@
       </c>
       <c r="F23" s="20"/>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="11">
         <v>23</v>
       </c>
@@ -4946,7 +5000,7 @@
       </c>
       <c r="F24" s="20"/>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="11">
         <v>24</v>
       </c>
@@ -4964,7 +5018,7 @@
       </c>
       <c r="F25" s="20"/>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="11">
         <v>25</v>
       </c>
@@ -4982,7 +5036,7 @@
       </c>
       <c r="F26" s="20"/>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="11">
         <v>26</v>
       </c>
@@ -5000,7 +5054,7 @@
       </c>
       <c r="F27" s="20"/>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="11">
         <v>27</v>
       </c>
@@ -5031,99 +5085,99 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="33" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="33.75">
-      <c r="A3" s="63"/>
-      <c r="B3" s="64" t="s">
+    <row r="3" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" s="59"/>
+      <c r="B3" s="60" t="s">
         <v>80</v>
       </c>
-      <c r="C3" s="64" t="s">
+      <c r="C3" s="60" t="s">
         <v>82</v>
       </c>
-      <c r="D3" s="65" t="s">
+      <c r="D3" s="61" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="102" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="97" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="103">
+      <c r="B4" s="98">
         <v>10</v>
       </c>
-      <c r="C4" s="72">
+      <c r="C4" s="67">
         <v>4</v>
       </c>
-      <c r="D4" s="72">
+      <c r="D4" s="67">
         <f>+B4*C4</f>
         <v>40</v>
       </c>
       <c r="E4" s="30"/>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="104" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="99" t="s">
         <v>75</v>
       </c>
-      <c r="B5" s="105">
+      <c r="B5" s="100">
         <v>9</v>
       </c>
-      <c r="C5" s="73">
+      <c r="C5" s="68">
         <v>4</v>
       </c>
-      <c r="D5" s="73">
+      <c r="D5" s="68">
         <f t="shared" ref="D5:D7" si="0">+B5*C5</f>
         <v>36</v>
       </c>
       <c r="E5" s="30"/>
     </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="104" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="99" t="s">
         <v>76</v>
       </c>
-      <c r="B6" s="105">
+      <c r="B6" s="100">
         <v>9</v>
       </c>
-      <c r="C6" s="73">
+      <c r="C6" s="68">
         <v>4</v>
       </c>
-      <c r="D6" s="73">
+      <c r="D6" s="68">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
       <c r="E6" s="30"/>
     </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="106" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="101" t="s">
         <v>77</v>
       </c>
-      <c r="B7" s="107">
+      <c r="B7" s="102">
         <v>6.9</v>
       </c>
-      <c r="C7" s="108">
+      <c r="C7" s="103">
         <v>18</v>
       </c>
-      <c r="D7" s="108">
+      <c r="D7" s="103">
         <f t="shared" si="0"/>
         <v>124.2</v>
       </c>
       <c r="E7" s="30"/>
     </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="67" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="63" t="s">
         <v>78</v>
       </c>
       <c r="B8" s="27">
@@ -5134,37 +5188,37 @@
         <f>+SUM(C4:C7)</f>
         <v>30</v>
       </c>
-      <c r="D8" s="109">
+      <c r="D8" s="104">
         <f>+SUM(D4:D7)</f>
         <v>236.2</v>
       </c>
       <c r="E8" s="30"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E9" s="30"/>
     </row>
-    <row r="10" spans="1:5">
-      <c r="B10" s="66" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B10" s="62" t="s">
         <v>41</v>
       </c>
       <c r="C10" s="8">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
-      <c r="B11" s="67" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B11" s="63" t="s">
         <v>79</v>
       </c>
-      <c r="C11" s="110">
+      <c r="C11" s="105">
         <f>+B8/C10</f>
         <v>8.7249999999999996</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="9.9499999999999993" customHeight="1">
+    <row r="12" spans="1:5" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
     </row>
-    <row r="13" spans="1:5" ht="18.75">
+    <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B13" s="32" t="s">
         <v>83</v>
       </c>
@@ -5172,11 +5226,11 @@
         <f>+D8</f>
         <v>236.2</v>
       </c>
-      <c r="D13" s="68" t="s">
+      <c r="D13" s="64" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="18.75">
+    <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B14" s="32" t="s">
         <v>84</v>
       </c>
@@ -5184,15 +5238,15 @@
         <f>+C8</f>
         <v>30</v>
       </c>
-      <c r="D14" s="68" t="s">
+      <c r="D14" s="64" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
-      <c r="B15" s="67" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B15" s="63" t="s">
         <v>93</v>
       </c>
-      <c r="C15" s="110">
+      <c r="C15" s="105">
         <f>+C13/C14</f>
         <v>7.8733333333333331</v>
       </c>
@@ -5205,196 +5259,289 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7576C37-4932-6048-BC1D-0E1FB524A1A8}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="4.83203125" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="45">
-      <c r="A2" s="42" t="s">
+    <row r="2" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+      <c r="A2" s="39" t="s">
         <v>85</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="42" t="s">
+      <c r="C2" s="39" t="s">
         <v>91</v>
       </c>
-      <c r="D2" s="42" t="s">
+      <c r="D2" s="39" t="s">
         <v>89</v>
       </c>
-      <c r="E2" s="42" t="s">
+      <c r="E2" s="110" t="s">
         <v>88</v>
       </c>
-      <c r="F2" s="42" t="s">
+      <c r="F2" s="39" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="42">
         <v>1</v>
       </c>
-      <c r="B3" s="46">
+      <c r="B3" s="43">
         <v>1000</v>
       </c>
-      <c r="C3" s="47">
+      <c r="C3" s="44">
         <v>4.6899999999999997E-2</v>
       </c>
-      <c r="D3" s="48">
+      <c r="D3" s="45">
         <f>+B3*C3</f>
         <v>46.9</v>
       </c>
-      <c r="E3" s="49">
+      <c r="E3" s="46">
         <f>+B3+D3</f>
         <v>1046.9000000000001</v>
       </c>
-      <c r="F3" s="50">
+      <c r="F3" s="47">
         <f>1+C3</f>
         <v>1.0468999999999999</v>
       </c>
-      <c r="G3" s="39"/>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="51">
+      <c r="G3" s="52"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="48">
         <v>2</v>
       </c>
-      <c r="B4" s="52">
+      <c r="B4" s="49">
         <f>+E3</f>
         <v>1046.9000000000001</v>
       </c>
-      <c r="C4" s="53">
-        <v>5.5E-2</v>
-      </c>
-      <c r="D4" s="54">
+      <c r="C4" s="116">
+        <v>-1.2E-2</v>
+      </c>
+      <c r="D4" s="51">
         <f>+B4*C4</f>
-        <v>57.579500000000003</v>
-      </c>
-      <c r="E4" s="55">
+        <v>-12.562800000000001</v>
+      </c>
+      <c r="E4" s="52">
         <f>+B4+D4</f>
-        <v>1104.4795000000001</v>
-      </c>
-      <c r="F4" s="56">
+        <v>1034.3372000000002</v>
+      </c>
+      <c r="F4" s="53">
         <f t="shared" ref="F4:F6" si="0">1+C4</f>
-        <v>1.0549999999999999</v>
-      </c>
-      <c r="G4" s="39"/>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="51">
+        <v>0.98799999999999999</v>
+      </c>
+      <c r="G4" s="52">
+        <f>+F3*F4</f>
+        <v>1.0343372</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="48">
         <v>3</v>
       </c>
-      <c r="B5" s="52">
+      <c r="B5" s="49">
         <f>+E4</f>
-        <v>1104.4795000000001</v>
-      </c>
-      <c r="C5" s="53">
+        <v>1034.3372000000002</v>
+      </c>
+      <c r="C5" s="50">
         <v>6.4199999999999993E-2</v>
       </c>
-      <c r="D5" s="54">
+      <c r="D5" s="51">
         <f>+B5*C5</f>
-        <v>70.907583900000006</v>
-      </c>
-      <c r="E5" s="55">
+        <v>66.404448240000008</v>
+      </c>
+      <c r="E5" s="52">
         <f>+B5+D5</f>
-        <v>1175.3870839000001</v>
-      </c>
-      <c r="F5" s="56">
+        <v>1100.7416482400001</v>
+      </c>
+      <c r="F5" s="53">
         <f t="shared" si="0"/>
         <v>1.0642</v>
       </c>
-      <c r="G5" s="39"/>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="57">
+      <c r="G5" s="52">
+        <f>+G4*F5</f>
+        <v>1.1007416482400001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="54">
         <v>4</v>
       </c>
-      <c r="B6" s="58">
+      <c r="B6" s="55">
         <f>+E5</f>
-        <v>1175.3870839000001</v>
-      </c>
-      <c r="C6" s="59">
+        <v>1100.7416482400001</v>
+      </c>
+      <c r="C6" s="56">
         <v>4.2700000000000002E-2</v>
       </c>
-      <c r="D6" s="60">
+      <c r="D6" s="57">
         <f>+B6*C6</f>
-        <v>50.189028482530006</v>
-      </c>
-      <c r="E6" s="61">
+        <v>47.001668379848006</v>
+      </c>
+      <c r="E6" s="115">
         <f>+B6+D6</f>
-        <v>1225.57611238253</v>
-      </c>
-      <c r="F6" s="62">
+        <v>1147.7433166198482</v>
+      </c>
+      <c r="F6" s="58">
         <f t="shared" si="0"/>
         <v>1.0427</v>
       </c>
-      <c r="G6" s="39"/>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="C8" s="44"/>
+      <c r="G6" s="112">
+        <f>+G5*F6</f>
+        <v>1.1477433166198481</v>
+      </c>
+      <c r="I6" s="3">
+        <f>+E6/B3*100-100</f>
+        <v>14.774331661984831</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C7" s="114">
+        <f>AVERAGE(C3:C6)</f>
+        <v>3.5449999999999995E-2</v>
+      </c>
+      <c r="I7" s="3">
+        <f>I6/4</f>
+        <v>3.6935829154962079</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C8" s="41"/>
       <c r="D8" s="18"/>
       <c r="E8" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="F8" s="44"/>
-      <c r="G8" s="39"/>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="F8" s="41"/>
+      <c r="G8" s="37"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G9" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="H9" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
       <c r="B10" s="34">
         <v>1000</v>
       </c>
-      <c r="C10" s="41"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="111"/>
+      <c r="C10" s="113">
+        <f>+H11-1</f>
+        <v>3.504967452483787E-2</v>
+      </c>
+      <c r="D10" s="3">
+        <f>+B10*C10</f>
+        <v>35.049674524837869</v>
+      </c>
+      <c r="E10" s="34">
+        <f>+B10+D10</f>
+        <v>1035.0496745248379</v>
+      </c>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2</v>
       </c>
-      <c r="B11" s="34"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="34"/>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="B11" s="34">
+        <f>+E10</f>
+        <v>1035.0496745248379</v>
+      </c>
+      <c r="C11" s="113">
+        <f>+C10</f>
+        <v>3.504967452483787E-2</v>
+      </c>
+      <c r="D11" s="3">
+        <f>+B11*C11</f>
+        <v>36.278154209134939</v>
+      </c>
+      <c r="E11" s="34">
+        <f>+B11+D11</f>
+        <v>1071.3278287339729</v>
+      </c>
+      <c r="G11" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="H11">
+        <f>G6^(1/4)</f>
+        <v>1.0350496745248379</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>3</v>
       </c>
-      <c r="B12" s="34"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="34"/>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="B12" s="34">
+        <f>+E11</f>
+        <v>1071.3278287339729</v>
+      </c>
+      <c r="C12" s="113">
+        <f>+C11</f>
+        <v>3.504967452483787E-2</v>
+      </c>
+      <c r="D12" s="3">
+        <f>+B12*C12</f>
+        <v>37.549691706527</v>
+      </c>
+      <c r="E12" s="34">
+        <f>+B12+D12</f>
+        <v>1108.8775204404999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>4</v>
       </c>
-      <c r="B13" s="34"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="34"/>
-    </row>
-    <row r="14" spans="1:7">
+      <c r="B13" s="34">
+        <f>+E12</f>
+        <v>1108.8775204404999</v>
+      </c>
+      <c r="C13" s="113">
+        <f>+C12</f>
+        <v>3.504967452483787E-2</v>
+      </c>
+      <c r="D13" s="3">
+        <f>+B13*C13</f>
+        <v>38.865796179348777</v>
+      </c>
+      <c r="E13" s="117">
+        <f>+B13+D13</f>
+        <v>1147.7433166198487</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E14" s="35"/>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B15" s="35"/>
-      <c r="D15" s="3"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="111"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5404,130 +5551,262 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B682753-6962-4871-9D9A-D4D9AA98E97D}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" zoomScale="240" zoomScaleNormal="240" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75">
-      <c r="A1" s="84" t="s">
+    <row r="1" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A1" s="79" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="45">
-      <c r="A2" s="75" t="s">
+    <row r="2" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+      <c r="A2" s="70" t="s">
         <v>99</v>
       </c>
-      <c r="B2" s="76" t="s">
+      <c r="B2" s="71" t="s">
         <v>96</v>
       </c>
-      <c r="C2" s="76" t="s">
+      <c r="C2" s="71" t="s">
         <v>97</v>
       </c>
-      <c r="D2" s="77" t="s">
+      <c r="D2" s="72" t="s">
+        <v>105</v>
+      </c>
+      <c r="G2" s="36" t="s">
+        <v>107</v>
+      </c>
+      <c r="H2" s="36" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="78" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="73" t="s">
         <v>98</v>
       </c>
-      <c r="B3" s="78">
+      <c r="B3" s="73">
         <v>90</v>
       </c>
-      <c r="C3" s="79">
+      <c r="C3" s="74">
         <f>1/B3</f>
         <v>1.1111111111111112E-2</v>
       </c>
-      <c r="D3" s="80"/>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="73" t="s">
+      <c r="D3" s="75">
+        <f>50/B3</f>
+        <v>0.55555555555555558</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="68" t="s">
         <v>98</v>
       </c>
-      <c r="B4" s="73">
+      <c r="B4" s="68">
         <v>70</v>
       </c>
-      <c r="C4" s="74">
-        <f t="shared" ref="C4:C7" si="0">1/B4</f>
+      <c r="C4" s="69">
+        <f>1/B4</f>
         <v>1.4285714285714285E-2</v>
       </c>
-      <c r="D4" s="54"/>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="73" t="s">
+      <c r="D4" s="51">
+        <f t="shared" ref="D4:D7" si="0">50/B4</f>
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="G4" s="118" t="s">
+        <v>109</v>
+      </c>
+      <c r="H4" s="118" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="68" t="s">
         <v>98</v>
       </c>
-      <c r="B5" s="73">
+      <c r="B5" s="68">
         <v>45</v>
       </c>
-      <c r="C5" s="74">
+      <c r="C5" s="69">
+        <f t="shared" ref="C4:C7" si="1">1/B5</f>
+        <v>2.2222222222222223E-2</v>
+      </c>
+      <c r="D5" s="51">
         <f t="shared" si="0"/>
-        <v>2.2222222222222223E-2</v>
-      </c>
-      <c r="D5" s="54"/>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="73" t="s">
+        <v>1.1111111111111112</v>
+      </c>
+      <c r="G5" s="11">
+        <v>1</v>
+      </c>
+      <c r="H5" s="119">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="68" t="s">
         <v>98</v>
       </c>
-      <c r="B6" s="73">
+      <c r="B6" s="68">
         <v>40</v>
       </c>
-      <c r="C6" s="74">
+      <c r="C6" s="69">
+        <f t="shared" si="1"/>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="D6" s="51">
         <f t="shared" si="0"/>
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="D6" s="54"/>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="81" t="s">
+        <v>1.25</v>
+      </c>
+      <c r="G6" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="H6" s="119">
+        <f>1/G6</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="76" t="s">
         <v>98</v>
       </c>
-      <c r="B7" s="81">
+      <c r="B7" s="76">
         <v>50</v>
       </c>
-      <c r="C7" s="82">
+      <c r="C7" s="77">
+        <f t="shared" si="1"/>
+        <v>0.02</v>
+      </c>
+      <c r="D7" s="78">
         <f t="shared" si="0"/>
-        <v>0.02</v>
-      </c>
-      <c r="D7" s="83"/>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="D8" s="11"/>
-    </row>
-    <row r="9" spans="1:4">
+        <v>1</v>
+      </c>
+      <c r="G7" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="H7" s="119">
+        <f>1/G7</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D8" s="17">
+        <f>+SUM(D3:D7)</f>
+        <v>4.6309523809523814</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="G8" s="11">
+        <v>0.01</v>
+      </c>
+      <c r="H8" s="119">
+        <f>1/G8</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D9" s="11"/>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="B10" s="67" t="s">
+      <c r="G9" s="11">
+        <v>1E-4</v>
+      </c>
+      <c r="H9" s="119">
+        <f>1/G9</f>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B10" s="63" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="40"/>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="B12" s="38"/>
-      <c r="C12" s="69"/>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="B13" s="38"/>
-      <c r="C13" s="38"/>
-    </row>
-    <row r="15" spans="1:4" ht="15.75">
-      <c r="B15" s="70" t="s">
+      <c r="C10" s="38">
+        <v>5</v>
+      </c>
+      <c r="G10" s="11">
+        <v>1.0000000000000001E-9</v>
+      </c>
+      <c r="H10" s="119">
+        <f>1/G10</f>
+        <v>999999999.99999988</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G11" s="11"/>
+      <c r="H11" s="119"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B12" s="108"/>
+      <c r="C12" s="109">
+        <f>+SUM(C3:C7)</f>
+        <v>9.2619047619047615E-2</v>
+      </c>
+      <c r="H12" s="119"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B13" s="108"/>
+      <c r="C13" s="108"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="119"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F14">
+        <v>50</v>
+      </c>
+      <c r="G14" s="11">
+        <v>100</v>
+      </c>
+      <c r="H14" s="119">
+        <f>+F14/G14</f>
+        <v>0.5</v>
+      </c>
+      <c r="I14" s="11">
+        <f>+H14*60</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="B15" s="65" t="s">
         <v>101</v>
       </c>
-      <c r="C15" s="71"/>
-    </row>
-    <row r="17" spans="3:3">
-      <c r="C17" s="3"/>
+      <c r="C15" s="66">
+        <f>+C10/C12</f>
+        <v>53.984575835475582</v>
+      </c>
+      <c r="D15" t="s">
+        <v>112</v>
+      </c>
+      <c r="F15">
+        <v>50</v>
+      </c>
+      <c r="G15" s="11">
+        <v>200</v>
+      </c>
+      <c r="H15" s="119">
+        <f>+F15/G15</f>
+        <v>0.25</v>
+      </c>
+      <c r="I15" s="11">
+        <f>+H15*60</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H16" s="35"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B17" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="C17" s="17">
+        <f>250/C15</f>
+        <v>4.6309523809523805</v>
+      </c>
+      <c r="H17" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>